<commit_message>
lecture 021 and 022 completed
</commit_message>
<xml_diff>
--- a/SIGMA_WEB_DEVELOPMENT_COURSE__CodeWithHarry_Lectures_Progress_Sheet.xlsx
+++ b/SIGMA_WEB_DEVELOPMENT_COURSE__CodeWithHarry_Lectures_Progress_Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\04_CodeWithHarry\SIGMA_WEB_DEVELOPMENT_Course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACDA231-A5A3-4D44-AB23-A973FCAD6396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2AAFC5-814E-45EB-A4A4-0E6998373171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
   <si>
     <t>Lectures</t>
   </si>
@@ -439,6 +439,21 @@
   </si>
   <si>
     <t>`-By CodeWithHarry (Youtube videos)</t>
+  </si>
+  <si>
+    <t>Video 132</t>
+  </si>
+  <si>
+    <t>Video 133</t>
+  </si>
+  <si>
+    <t>Video 134</t>
+  </si>
+  <si>
+    <t>Video 135</t>
+  </si>
+  <si>
+    <t>Video 136</t>
   </si>
 </sst>
 </file>
@@ -820,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:M209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10:F27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,7 +1091,7 @@
         <v>20</v>
       </c>
       <c r="F28" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="4:6" ht="33.75" x14ac:dyDescent="0.5">
@@ -1084,7 +1099,7 @@
         <v>21</v>
       </c>
       <c r="F29" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="4:6" ht="33.75" x14ac:dyDescent="0.5">
@@ -1092,7 +1107,7 @@
         <v>22</v>
       </c>
       <c r="F30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="4:6" ht="33.75" x14ac:dyDescent="0.5">
@@ -1100,7 +1115,7 @@
         <v>23</v>
       </c>
       <c r="F31" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="4:6" ht="33.75" x14ac:dyDescent="0.5">
@@ -1976,24 +1991,44 @@
       </c>
     </row>
     <row r="141" spans="4:6" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="D141" s="4"/>
-      <c r="F141" s="5"/>
+      <c r="D141" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F141" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="142" spans="4:6" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="D142" s="4"/>
-      <c r="F142" s="5"/>
+      <c r="D142" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F142" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="143" spans="4:6" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="D143" s="4"/>
-      <c r="F143" s="5"/>
+      <c r="D143" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F143" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="144" spans="4:6" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="D144" s="4"/>
-      <c r="F144" s="5"/>
+      <c r="D144" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F144" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="145" spans="4:6" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="D145" s="4"/>
-      <c r="F145" s="5"/>
+      <c r="D145" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F145" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="146" spans="4:6" ht="33.75" x14ac:dyDescent="0.5">
       <c r="D146" s="4"/>

</xml_diff>